<commit_message>
updated results and README
</commit_message>
<xml_diff>
--- a/backprop.xlsx
+++ b/backprop.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22356" windowHeight="9935"/>
+    <workbookView windowWidth="18455" windowHeight="9935" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="training" sheetId="1" r:id="rId1"/>
+    <sheet name="lr_charts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>Equations for foward pass</t>
   </si>
@@ -280,16 +281,19 @@
   <si>
     <t>∂E2/∂a_o2</t>
   </si>
+  <si>
+    <t>Total Error</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -313,6 +317,29 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -323,14 +350,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -352,7 +371,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -361,14 +380,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -390,6 +401,14 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -406,7 +425,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -415,14 +434,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -436,22 +448,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -508,6 +512,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -520,49 +530,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,7 +566,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,7 +584,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,25 +626,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,7 +650,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -646,25 +662,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -676,13 +680,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,6 +697,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -711,6 +730,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -722,17 +750,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -770,26 +787,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -798,154 +802,157 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
@@ -977,9 +984,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -995,17 +999,11 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
@@ -1069,6 +1067,1556 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr defTabSz="914400">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>Impact of Learning Rate</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lr_charts!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>lr_charts!$B$3:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.242519857348377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.241109038768129</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.239704031568673</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.238304879953206</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.236911627306511</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.235524316174669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.234142988245484</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.232767684329637</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.231398444342584</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.230035307287211</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22867831123726</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.227327493321532</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.225982889708882</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.224644535594015</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.223312465184083</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.221986711686093</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.220667307295137</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.219354283183434</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.218047669490196</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.216747495312321</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.215453788695897</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lr_charts!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>lr_charts!$C$3:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.242519857348377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.239701143428983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.236905839125625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.234134290206886</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.231386828822159</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.228663772898847</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.225965425587682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.223292074757764</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.220643992542521</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.218021434937551</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.215424641450897</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.212853834806064</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.210309220697726</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.207790987599822</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.205299306625418</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.20283433143748</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.200396198209435</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.197985025634177</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.195600914979954</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.193243950191404</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.190914198033808</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lr_charts!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>lr_charts!$D$3:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.242519857348377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23549537787349</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.228620206008707</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.221899352900572</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.215337243557067</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.208937672741089</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.202703773668297</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.196637999599531</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.190742117970789</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1850172163143</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.179463718906352</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.174081412839012</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.168869482055565</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.163826547810226</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.158950714004049</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.154239615900672</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.149690470825535</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.145300129587915</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.141065127524268</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.136981734232741</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.13304600124279</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lr_charts!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>lr_charts!$E$3:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.242519857348377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.231317286429774</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.220504294375079</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.210099675846141</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.200118107279643</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.190569848840512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.181460660049517</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.172791911600233</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.164560862432118</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.156761063111352</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.149382843878267</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.142413847503562</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.135839572094707</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.129643895849052</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.12380956324187</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.118318619327559</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.113152785108043</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.108293771973121</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.103723536970209</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0994244832049085</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0953796111899922</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lr_charts!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>lr_charts!$F$3:$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.242519857348377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.228547765278785</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.215191751301094</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.202486151516938</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.190454908237779</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17911099514393</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.168456619893661</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.158484073157016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.149177040363366</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.140512178869125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.132460780886447</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.124990379392256</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.118066198452389</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.111652391770278</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.105713048301803</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.100212969309595</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0951182374839108</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0903966072783703</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0860177484159392</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0819533735590565</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0781772780087398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lr_charts!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>lr_charts!$G$3:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.242519857348377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.214901598842566</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.189879326144002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16762535191282</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.148139495080156</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.131275319676479</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11678987307369</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.104394940528933</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.093796722981055</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.084720552415379</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0769229799763193</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0701953307329663</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0643623981427226</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0592788523891631</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0548249102793957</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0509020835134517</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0474293724702455</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0443400238332432</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0415788462218575</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0391000243910868</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0368653558893979</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="497410531"/>
+        <c:axId val="56163900"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="497410531"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr defTabSz="914400">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>Epochs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="56163900"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="56163900"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr defTabSz="914400">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="497410531"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-US"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5638,6 +7186,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>294640</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>93980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>599440</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>93980</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6024880" y="1374140"/>
+        <a:ext cx="4572000" cy="2743200"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -5898,8 +7481,8 @@
   <sheetPr/>
   <dimension ref="A5:AQ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AH18" sqref="AH18"/>
+    <sheetView zoomScale="86" zoomScaleNormal="86" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35:P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.52777777777778" defaultRowHeight="14.4"/>
@@ -5971,7 +7554,7 @@
       </c>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -6031,7 +7614,7 @@
       </c>
     </row>
     <row r="27" spans="19:19">
-      <c r="S27" s="7"/>
+      <c r="S27" s="8"/>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
@@ -6059,34 +7642,34 @@
       </c>
     </row>
     <row r="34" spans="16:16">
-      <c r="P34" s="7">
+      <c r="P34" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:41">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="4" t="s">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="8" t="s">
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="10" t="s">
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="11" t="s">
         <v>34</v>
       </c>
       <c r="R35" s="11"/>
@@ -6100,73 +7683,73 @@
       <c r="X35" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="Y35" s="17"/>
-      <c r="Z35" s="17"/>
-      <c r="AA35" s="17"/>
-      <c r="AB35" s="17"/>
-      <c r="AC35" s="17"/>
-      <c r="AD35" s="17"/>
-      <c r="AE35" s="17"/>
-      <c r="AF35" s="18" t="s">
+      <c r="Y35" s="13"/>
+      <c r="Z35" s="13"/>
+      <c r="AA35" s="13"/>
+      <c r="AB35" s="13"/>
+      <c r="AC35" s="13"/>
+      <c r="AD35" s="13"/>
+      <c r="AE35" s="13"/>
+      <c r="AF35" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="AG35" s="20"/>
-      <c r="AH35" s="20"/>
-      <c r="AI35" s="20"/>
-      <c r="AJ35" s="20"/>
-      <c r="AK35" s="20"/>
-      <c r="AL35" s="20"/>
-      <c r="AM35" s="20"/>
-      <c r="AN35" s="20"/>
-      <c r="AO35" s="20"/>
+      <c r="AG35" s="17"/>
+      <c r="AH35" s="17"/>
+      <c r="AI35" s="17"/>
+      <c r="AJ35" s="17"/>
+      <c r="AK35" s="17"/>
+      <c r="AL35" s="17"/>
+      <c r="AM35" s="17"/>
+      <c r="AN35" s="17"/>
+      <c r="AO35" s="17"/>
     </row>
-    <row r="36" s="1" customFormat="1" spans="1:43">
-      <c r="A36" s="5" t="s">
+    <row r="36" s="2" customFormat="1" spans="1:43">
+      <c r="A36" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="G36" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="I36" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J36" s="6" t="s">
+      <c r="J36" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="K36" s="6" t="s">
+      <c r="K36" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="L36" s="6" t="s">
+      <c r="L36" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M36" s="9" t="s">
+      <c r="M36" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="N36" s="9" t="s">
+      <c r="N36" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="O36" s="9" t="s">
+      <c r="O36" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="P36" s="9" t="s">
+      <c r="P36" s="10" t="s">
         <v>53</v>
       </c>
       <c r="Q36" s="14" t="s">
@@ -6214,38 +7797,38 @@
       <c r="AE36" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="AF36" s="19" t="s">
+      <c r="AF36" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="AG36" s="19" t="s">
+      <c r="AG36" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="AH36" s="19" t="s">
+      <c r="AH36" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="AI36" s="19" t="s">
+      <c r="AI36" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="AJ36" s="19" t="s">
+      <c r="AJ36" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="AK36" s="19" t="s">
+      <c r="AK36" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="AL36" s="19" t="s">
+      <c r="AL36" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="AM36" s="19" t="s">
+      <c r="AM36" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="AN36" s="19" t="s">
+      <c r="AN36" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="AO36" s="19" t="s">
+      <c r="AO36" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="AP36" s="21"/>
-      <c r="AQ36" s="21"/>
+      <c r="AP36" s="19"/>
+      <c r="AQ36" s="19"/>
     </row>
     <row r="37" spans="1:41">
       <c r="A37">
@@ -6504,7 +8087,7 @@
       </c>
       <c r="AA38">
         <f>(AN38*AL38*AI38*AG38+AO38*AM38*AK38*AG38)*B38</f>
-        <v>0.000288269090809018</v>
+        <v>0.000288269090809017</v>
       </c>
       <c r="AB38">
         <f>AN38*AL38*N38</f>
@@ -6662,7 +8245,7 @@
       </c>
       <c r="Z39">
         <f t="shared" ref="Z39:Z57" si="22">(AN39*AL39*AI39*AG39+AO39*AM39*AK39*AG39)*A39</f>
-        <v>6.53288389525536e-5</v>
+        <v>6.53288389525534e-5</v>
       </c>
       <c r="AA39">
         <f t="shared" ref="AA39:AA57" si="23">(AN39*AL39*AI39*AG39+AO39*AM39*AK39*AG39)*B39</f>
@@ -6824,11 +8407,11 @@
       </c>
       <c r="Z40">
         <f t="shared" si="22"/>
-        <v>-1.14340553421902e-5</v>
+        <v>-1.14340553421906e-5</v>
       </c>
       <c r="AA40">
         <f t="shared" si="23"/>
-        <v>-2.28681106843804e-5</v>
+        <v>-2.28681106843811e-5</v>
       </c>
       <c r="AB40">
         <f t="shared" si="24"/>
@@ -6986,11 +8569,11 @@
       </c>
       <c r="Z41">
         <f t="shared" si="22"/>
-        <v>-8.59977837089744e-5</v>
+        <v>-8.59977837089748e-5</v>
       </c>
       <c r="AA41">
         <f t="shared" si="23"/>
-        <v>-0.000171995567417949</v>
+        <v>-0.00017199556741795</v>
       </c>
       <c r="AB41">
         <f t="shared" si="24"/>
@@ -7084,7 +8667,7 @@
       </c>
       <c r="J42">
         <f t="shared" si="6"/>
-        <v>0.271254362876523</v>
+        <v>0.271254362876522</v>
       </c>
       <c r="K42">
         <f t="shared" si="7"/>
@@ -7092,7 +8675,7 @@
       </c>
       <c r="L42">
         <f t="shared" si="8"/>
-        <v>0.652810425593925</v>
+        <v>0.652810425593926</v>
       </c>
       <c r="M42">
         <f t="shared" si="9"/>
@@ -7148,7 +8731,7 @@
       </c>
       <c r="Z42">
         <f t="shared" si="22"/>
-        <v>-0.000158221350407709</v>
+        <v>-0.00015822135040771</v>
       </c>
       <c r="AA42">
         <f t="shared" si="23"/>
@@ -7184,7 +8767,7 @@
       </c>
       <c r="AI42">
         <f t="shared" si="31"/>
-        <v>0.271254362876523</v>
+        <v>0.271254362876522</v>
       </c>
       <c r="AJ42">
         <f t="shared" si="32"/>
@@ -7192,7 +8775,7 @@
       </c>
       <c r="AK42">
         <f t="shared" si="33"/>
-        <v>0.652810425593925</v>
+        <v>0.652810425593926</v>
       </c>
       <c r="AL42">
         <f t="shared" si="34"/>
@@ -7314,7 +8897,7 @@
       </c>
       <c r="AA43">
         <f t="shared" si="23"/>
-        <v>-0.000455961577284892</v>
+        <v>-0.000455961577284893</v>
       </c>
       <c r="AB43">
         <f t="shared" si="24"/>
@@ -7448,7 +9031,7 @@
       </c>
       <c r="T44">
         <f t="shared" si="16"/>
-        <v>0.663163334600139</v>
+        <v>0.66316333460014</v>
       </c>
       <c r="U44">
         <f t="shared" si="17"/>
@@ -7464,15 +9047,15 @@
       </c>
       <c r="X44">
         <f t="shared" si="20"/>
-        <v>-0.000328594663640638</v>
+        <v>-0.000328594663640637</v>
       </c>
       <c r="Y44">
         <f t="shared" si="21"/>
-        <v>-0.000657189327281275</v>
+        <v>-0.000657189327281274</v>
       </c>
       <c r="Z44">
         <f t="shared" si="22"/>
-        <v>-0.000295170371982814</v>
+        <v>-0.000295170371982813</v>
       </c>
       <c r="AA44">
         <f t="shared" si="23"/>
@@ -7532,7 +9115,7 @@
       </c>
       <c r="AO44">
         <f t="shared" si="37"/>
-        <v>-0.326836665399861</v>
+        <v>-0.32683666539986</v>
       </c>
     </row>
     <row r="45" spans="1:41">
@@ -7638,7 +9221,7 @@
       </c>
       <c r="AA45">
         <f t="shared" si="23"/>
-        <v>-0.000719406730745506</v>
+        <v>-0.000719406730745507</v>
       </c>
       <c r="AB45">
         <f t="shared" si="24"/>
@@ -7800,7 +9383,7 @@
       </c>
       <c r="AA46">
         <f t="shared" si="23"/>
-        <v>-0.000843024664139846</v>
+        <v>-0.000843024664139847</v>
       </c>
       <c r="AB46">
         <f t="shared" si="24"/>
@@ -8056,7 +9639,7 @@
       </c>
       <c r="J48">
         <f t="shared" si="6"/>
-        <v>0.0694418103435464</v>
+        <v>0.0694418103435463</v>
       </c>
       <c r="K48">
         <f t="shared" si="7"/>
@@ -8120,7 +9703,7 @@
       </c>
       <c r="Z48">
         <f t="shared" si="22"/>
-        <v>-0.000536783922562964</v>
+        <v>-0.000536783922562965</v>
       </c>
       <c r="AA48">
         <f t="shared" si="23"/>
@@ -8156,7 +9739,7 @@
       </c>
       <c r="AI48">
         <f t="shared" si="31"/>
-        <v>0.0694418103435464</v>
+        <v>0.0694418103435463</v>
       </c>
       <c r="AJ48">
         <f t="shared" si="32"/>
@@ -8218,7 +9801,7 @@
       </c>
       <c r="J49">
         <f t="shared" si="6"/>
-        <v>0.0374348901391421</v>
+        <v>0.037434890139142</v>
       </c>
       <c r="K49">
         <f t="shared" si="7"/>
@@ -8318,7 +9901,7 @@
       </c>
       <c r="AI49">
         <f t="shared" si="31"/>
-        <v>0.0374348901391421</v>
+        <v>0.037434890139142</v>
       </c>
       <c r="AJ49">
         <f t="shared" si="32"/>
@@ -8380,7 +9963,7 @@
       </c>
       <c r="J50">
         <f t="shared" si="6"/>
-        <v>0.00592880874127213</v>
+        <v>0.00592880874127202</v>
       </c>
       <c r="K50">
         <f t="shared" si="7"/>
@@ -8408,7 +9991,7 @@
       </c>
       <c r="Q50">
         <f t="shared" si="13"/>
-        <v>-0.0176650355527502</v>
+        <v>-0.0176650355527503</v>
       </c>
       <c r="R50">
         <f t="shared" si="14"/>
@@ -8480,7 +10063,7 @@
       </c>
       <c r="AI50">
         <f t="shared" si="31"/>
-        <v>0.00592880874127213</v>
+        <v>0.00592880874127202</v>
       </c>
       <c r="AJ50">
         <f t="shared" si="32"/>
@@ -8542,7 +10125,7 @@
       </c>
       <c r="J51">
         <f t="shared" si="6"/>
-        <v>-0.0250677652102679</v>
+        <v>-0.025067765210268</v>
       </c>
       <c r="K51">
         <f t="shared" si="7"/>
@@ -8550,7 +10133,7 @@
       </c>
       <c r="L51">
         <f t="shared" si="8"/>
-        <v>0.814534811430703</v>
+        <v>0.814534811430704</v>
       </c>
       <c r="M51">
         <f t="shared" si="9"/>
@@ -8570,7 +10153,7 @@
       </c>
       <c r="Q51">
         <f t="shared" si="13"/>
-        <v>-0.0490967744483688</v>
+        <v>-0.0490967744483689</v>
       </c>
       <c r="R51">
         <f t="shared" si="14"/>
@@ -8642,7 +10225,7 @@
       </c>
       <c r="AI51">
         <f t="shared" si="31"/>
-        <v>-0.0250677652102679</v>
+        <v>-0.025067765210268</v>
       </c>
       <c r="AJ51">
         <f t="shared" si="32"/>
@@ -8650,7 +10233,7 @@
       </c>
       <c r="AK51">
         <f t="shared" si="33"/>
-        <v>0.814534811430703</v>
+        <v>0.814534811430704</v>
       </c>
       <c r="AL51">
         <f t="shared" si="34"/>
@@ -8704,7 +10287,7 @@
       </c>
       <c r="J52">
         <f t="shared" si="6"/>
-        <v>-0.0555480913259863</v>
+        <v>-0.0555480913259864</v>
       </c>
       <c r="K52">
         <f t="shared" si="7"/>
@@ -8768,7 +10351,7 @@
       </c>
       <c r="Z52">
         <f t="shared" si="22"/>
-        <v>-0.000733718408548969</v>
+        <v>-0.00073371840854897</v>
       </c>
       <c r="AA52">
         <f t="shared" si="23"/>
@@ -8804,7 +10387,7 @@
       </c>
       <c r="AI52">
         <f t="shared" si="31"/>
-        <v>-0.0555480913259863</v>
+        <v>-0.0555480913259864</v>
       </c>
       <c r="AJ52">
         <f t="shared" si="32"/>
@@ -8866,7 +10449,7 @@
       </c>
       <c r="J53">
         <f t="shared" si="6"/>
-        <v>-0.0855072583132153</v>
+        <v>-0.0855072583132154</v>
       </c>
       <c r="K53">
         <f t="shared" si="7"/>
@@ -8874,7 +10457,7 @@
       </c>
       <c r="L53">
         <f t="shared" si="8"/>
-        <v>0.846922921240431</v>
+        <v>0.846922921240432</v>
       </c>
       <c r="M53">
         <f t="shared" si="9"/>
@@ -8930,7 +10513,7 @@
       </c>
       <c r="Z53">
         <f t="shared" si="22"/>
-        <v>-0.000776087444255236</v>
+        <v>-0.000776087444255237</v>
       </c>
       <c r="AA53">
         <f t="shared" si="23"/>
@@ -8966,7 +10549,7 @@
       </c>
       <c r="AI53">
         <f t="shared" si="31"/>
-        <v>-0.0855072583132153</v>
+        <v>-0.0855072583132154</v>
       </c>
       <c r="AJ53">
         <f t="shared" si="32"/>
@@ -8974,7 +10557,7 @@
       </c>
       <c r="AK53">
         <f t="shared" si="33"/>
-        <v>0.846922921240431</v>
+        <v>0.846922921240432</v>
       </c>
       <c r="AL53">
         <f t="shared" si="34"/>
@@ -9190,7 +10773,7 @@
       </c>
       <c r="J55">
         <f t="shared" si="6"/>
-        <v>-0.143850955330637</v>
+        <v>-0.143850955330638</v>
       </c>
       <c r="K55">
         <f t="shared" si="7"/>
@@ -9290,7 +10873,7 @@
       </c>
       <c r="AI55">
         <f t="shared" si="31"/>
-        <v>-0.143850955330637</v>
+        <v>-0.143850955330638</v>
       </c>
       <c r="AJ55">
         <f t="shared" si="32"/>
@@ -9352,7 +10935,7 @@
       </c>
       <c r="J56">
         <f t="shared" si="6"/>
-        <v>-0.172233796802239</v>
+        <v>-0.17223379680224</v>
       </c>
       <c r="K56">
         <f t="shared" si="7"/>
@@ -9452,7 +11035,7 @@
       </c>
       <c r="AI56">
         <f t="shared" si="31"/>
-        <v>-0.172233796802239</v>
+        <v>-0.17223379680224</v>
       </c>
       <c r="AJ56">
         <f t="shared" si="32"/>
@@ -9655,4 +11238,482 @@
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="2" width="13.1111111111111" customWidth="1"/>
+    <col min="6" max="6" width="12.8888888888889"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7">
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <v>0.2</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>0.8</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3">
+        <v>0.242519857348377</v>
+      </c>
+      <c r="C3">
+        <v>0.242519857348377</v>
+      </c>
+      <c r="D3">
+        <v>0.242519857348377</v>
+      </c>
+      <c r="E3">
+        <v>0.242519857348377</v>
+      </c>
+      <c r="F3">
+        <v>0.242519857348377</v>
+      </c>
+      <c r="G3">
+        <v>0.242519857348377</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4">
+        <v>0.241109038768129</v>
+      </c>
+      <c r="C4">
+        <v>0.239701143428983</v>
+      </c>
+      <c r="D4">
+        <v>0.23549537787349</v>
+      </c>
+      <c r="E4">
+        <v>0.231317286429774</v>
+      </c>
+      <c r="F4">
+        <v>0.228547765278785</v>
+      </c>
+      <c r="G4">
+        <v>0.214901598842566</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5">
+        <v>0.239704031568673</v>
+      </c>
+      <c r="C5">
+        <v>0.236905839125625</v>
+      </c>
+      <c r="D5">
+        <v>0.228620206008707</v>
+      </c>
+      <c r="E5">
+        <v>0.220504294375079</v>
+      </c>
+      <c r="F5">
+        <v>0.215191751301094</v>
+      </c>
+      <c r="G5">
+        <v>0.189879326144002</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6">
+        <v>0.238304879953206</v>
+      </c>
+      <c r="C6">
+        <v>0.234134290206886</v>
+      </c>
+      <c r="D6">
+        <v>0.221899352900572</v>
+      </c>
+      <c r="E6">
+        <v>0.210099675846141</v>
+      </c>
+      <c r="F6">
+        <v>0.202486151516938</v>
+      </c>
+      <c r="G6">
+        <v>0.16762535191282</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7">
+        <v>0.236911627306511</v>
+      </c>
+      <c r="C7">
+        <v>0.231386828822159</v>
+      </c>
+      <c r="D7">
+        <v>0.215337243557067</v>
+      </c>
+      <c r="E7">
+        <v>0.200118107279643</v>
+      </c>
+      <c r="F7">
+        <v>0.190454908237779</v>
+      </c>
+      <c r="G7">
+        <v>0.148139495080156</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8">
+        <v>0.235524316174669</v>
+      </c>
+      <c r="C8">
+        <v>0.228663772898847</v>
+      </c>
+      <c r="D8">
+        <v>0.208937672741089</v>
+      </c>
+      <c r="E8">
+        <v>0.190569848840512</v>
+      </c>
+      <c r="F8">
+        <v>0.17911099514393</v>
+      </c>
+      <c r="G8">
+        <v>0.131275319676479</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9">
+        <v>0.234142988245484</v>
+      </c>
+      <c r="C9">
+        <v>0.225965425587682</v>
+      </c>
+      <c r="D9">
+        <v>0.202703773668297</v>
+      </c>
+      <c r="E9">
+        <v>0.181460660049517</v>
+      </c>
+      <c r="F9">
+        <v>0.168456619893661</v>
+      </c>
+      <c r="G9">
+        <v>0.11678987307369</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10">
+        <v>0.232767684329637</v>
+      </c>
+      <c r="C10">
+        <v>0.223292074757764</v>
+      </c>
+      <c r="D10">
+        <v>0.196637999599531</v>
+      </c>
+      <c r="E10">
+        <v>0.172791911600233</v>
+      </c>
+      <c r="F10">
+        <v>0.158484073157016</v>
+      </c>
+      <c r="G10">
+        <v>0.104394940528933</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11">
+        <v>0.231398444342584</v>
+      </c>
+      <c r="C11">
+        <v>0.220643992542521</v>
+      </c>
+      <c r="D11">
+        <v>0.190742117970789</v>
+      </c>
+      <c r="E11">
+        <v>0.164560862432118</v>
+      </c>
+      <c r="F11">
+        <v>0.149177040363366</v>
+      </c>
+      <c r="G11">
+        <v>0.093796722981055</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12">
+        <v>0.230035307287211</v>
+      </c>
+      <c r="C12">
+        <v>0.218021434937551</v>
+      </c>
+      <c r="D12">
+        <v>0.1850172163143</v>
+      </c>
+      <c r="E12">
+        <v>0.156761063111352</v>
+      </c>
+      <c r="F12">
+        <v>0.140512178869125</v>
+      </c>
+      <c r="G12">
+        <v>0.084720552415379</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13">
+        <v>0.22867831123726</v>
+      </c>
+      <c r="C13">
+        <v>0.215424641450897</v>
+      </c>
+      <c r="D13">
+        <v>0.179463718906352</v>
+      </c>
+      <c r="E13">
+        <v>0.149382843878267</v>
+      </c>
+      <c r="F13">
+        <v>0.132460780886447</v>
+      </c>
+      <c r="G13">
+        <v>0.0769229799763193</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14">
+        <v>0.227327493321532</v>
+      </c>
+      <c r="C14">
+        <v>0.212853834806064</v>
+      </c>
+      <c r="D14">
+        <v>0.174081412839012</v>
+      </c>
+      <c r="E14">
+        <v>0.142413847503562</v>
+      </c>
+      <c r="F14">
+        <v>0.124990379392256</v>
+      </c>
+      <c r="G14">
+        <v>0.0701953307329663</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15">
+        <v>0.225982889708882</v>
+      </c>
+      <c r="C15">
+        <v>0.210309220697726</v>
+      </c>
+      <c r="D15">
+        <v>0.168869482055565</v>
+      </c>
+      <c r="E15">
+        <v>0.135839572094707</v>
+      </c>
+      <c r="F15">
+        <v>0.118066198452389</v>
+      </c>
+      <c r="G15">
+        <v>0.0643623981427226</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16">
+        <v>0.224644535594015</v>
+      </c>
+      <c r="C16">
+        <v>0.207790987599822</v>
+      </c>
+      <c r="D16">
+        <v>0.163826547810226</v>
+      </c>
+      <c r="E16">
+        <v>0.129643895849052</v>
+      </c>
+      <c r="F16">
+        <v>0.111652391770278</v>
+      </c>
+      <c r="G16">
+        <v>0.0592788523891631</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17">
+        <v>0.223312465184083</v>
+      </c>
+      <c r="C17">
+        <v>0.205299306625418</v>
+      </c>
+      <c r="D17">
+        <v>0.158950714004049</v>
+      </c>
+      <c r="E17">
+        <v>0.12380956324187</v>
+      </c>
+      <c r="F17">
+        <v>0.105713048301803</v>
+      </c>
+      <c r="G17">
+        <v>0.0548249102793957</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18">
+        <v>0.221986711686093</v>
+      </c>
+      <c r="C18">
+        <v>0.20283433143748</v>
+      </c>
+      <c r="D18">
+        <v>0.154239615900672</v>
+      </c>
+      <c r="E18">
+        <v>0.118318619327559</v>
+      </c>
+      <c r="F18">
+        <v>0.100212969309595</v>
+      </c>
+      <c r="G18">
+        <v>0.0509020835134517</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19">
+        <v>0.220667307295137</v>
+      </c>
+      <c r="C19">
+        <v>0.200396198209435</v>
+      </c>
+      <c r="D19">
+        <v>0.149690470825535</v>
+      </c>
+      <c r="E19">
+        <v>0.113152785108043</v>
+      </c>
+      <c r="F19">
+        <v>0.0951182374839108</v>
+      </c>
+      <c r="G19">
+        <v>0.0474293724702455</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20">
+        <v>0.219354283183434</v>
+      </c>
+      <c r="C20">
+        <v>0.197985025634177</v>
+      </c>
+      <c r="D20">
+        <v>0.145300129587915</v>
+      </c>
+      <c r="E20">
+        <v>0.108293771973121</v>
+      </c>
+      <c r="F20">
+        <v>0.0903966072783703</v>
+      </c>
+      <c r="G20">
+        <v>0.0443400238332432</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21">
+        <v>0.218047669490196</v>
+      </c>
+      <c r="C21">
+        <v>0.195600914979954</v>
+      </c>
+      <c r="D21">
+        <v>0.141065127524268</v>
+      </c>
+      <c r="E21">
+        <v>0.103723536970209</v>
+      </c>
+      <c r="F21">
+        <v>0.0860177484159392</v>
+      </c>
+      <c r="G21">
+        <v>0.0415788462218575</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22">
+        <v>0.216747495312321</v>
+      </c>
+      <c r="C22">
+        <v>0.193243950191404</v>
+      </c>
+      <c r="D22">
+        <v>0.136981734232741</v>
+      </c>
+      <c r="E22">
+        <v>0.0994244832049085</v>
+      </c>
+      <c r="F22">
+        <v>0.0819533735590565</v>
+      </c>
+      <c r="G22">
+        <v>0.0391000243910868</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23">
+        <v>0.215453788695897</v>
+      </c>
+      <c r="C23">
+        <v>0.190914198033808</v>
+      </c>
+      <c r="D23">
+        <v>0.13304600124279</v>
+      </c>
+      <c r="E23">
+        <v>0.0953796111899922</v>
+      </c>
+      <c r="F23">
+        <v>0.0781772780087398</v>
+      </c>
+      <c r="G23">
+        <v>0.0368653558893979</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>